<commit_message>
add x264 support and clean files
</commit_message>
<xml_diff>
--- a/ImageFormat_SourceCode/设置/setting_video.xlsx
+++ b/ImageFormat_SourceCode/设置/setting_video.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC0694B-32F2-466B-8C8E-A82170A77220}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317CE4AE-6C77-4584-A4C3-C6A1ACD599D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="61">
   <si>
     <t>源文件名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -240,6 +240,26 @@
   </si>
   <si>
     <t>https://github.com/webmproject/libvpx/releases</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVC(H264)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISO/ITU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>version n4.3.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/FFmpeg/Ffmpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FFMPEG</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -409,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,6 +494,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -493,6 +516,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -781,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409A2C8A-2D12-4E48-8DAB-3C644ED314BB}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -832,210 +861,232 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="21">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="4">
+        <v>44023</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="28"/>
+      <c r="B4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C4" s="18">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4" s="10" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
+      <c r="B5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C5" s="10">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F5" s="4">
         <v>44056</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C6" s="10">
         <v>3</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F6" s="4">
         <v>44097</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C7" s="18">
         <v>4</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F7" s="4">
         <v>43969</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
+      <c r="B8" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C8" s="18">
         <v>5</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F8" s="4">
         <v>44083</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="22"/>
+      <c r="B9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C9" s="18">
         <v>6</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F9" s="4">
         <v>44081</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B10" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C10" s="18">
         <v>7</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F10" s="4">
         <v>44043</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="19" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
+      <c r="B11" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C11" s="18">
         <v>8</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F11" s="4">
         <v>44034</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{13364C8A-E4FD-42A7-B997-43341ECC7128}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{84FD8E44-4AA8-4F69-B053-35F4B91A3B65}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{3EA407F3-CB2D-44FB-BAF1-7D615C160D3D}"/>
-    <hyperlink ref="G6" r:id="rId4" xr:uid="{6696EDD2-5D33-4EA2-9B2F-C75EEE4E8731}"/>
-    <hyperlink ref="G7" r:id="rId5" xr:uid="{8F813257-0137-41B7-AEE2-70E12407F464}"/>
-    <hyperlink ref="G8" r:id="rId6" xr:uid="{560B0781-9375-4481-A487-C16B5E041E10}"/>
-    <hyperlink ref="G10" r:id="rId7" xr:uid="{9DA675A7-EE1D-472C-9BB6-F8E5C2FF820E}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{0AC45F3F-841A-4754-9E4D-2EEE72218717}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{13364C8A-E4FD-42A7-B997-43341ECC7128}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{84FD8E44-4AA8-4F69-B053-35F4B91A3B65}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{3EA407F3-CB2D-44FB-BAF1-7D615C160D3D}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{6696EDD2-5D33-4EA2-9B2F-C75EEE4E8731}"/>
+    <hyperlink ref="G8" r:id="rId5" xr:uid="{8F813257-0137-41B7-AEE2-70E12407F464}"/>
+    <hyperlink ref="G9" r:id="rId6" xr:uid="{560B0781-9375-4481-A487-C16B5E041E10}"/>
+    <hyperlink ref="G11" r:id="rId7" xr:uid="{9DA675A7-EE1D-472C-9BB6-F8E5C2FF820E}"/>
+    <hyperlink ref="G10" r:id="rId8" xr:uid="{0AC45F3F-841A-4754-9E4D-2EEE72218717}"/>
+    <hyperlink ref="G3" r:id="rId9" xr:uid="{C5B0A1C3-07C0-47AC-A10F-2CAC97659866}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE997EE-6AF0-45C6-96DA-238F98F10E6B}">
-  <dimension ref="A1:O126"/>
+  <dimension ref="A1:O127"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="L3" sqref="L3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1062,30 +1113,30 @@
       <c r="C1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="25"/>
       <c r="H1" s="11"/>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="26" t="s">
         <v>19</v>
       </c>
       <c r="K1" s="11"/>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22" t="s">
+      <c r="M1" s="23"/>
+      <c r="N1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="22"/>
+      <c r="O1" s="23"/>
     </row>
     <row r="2" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
@@ -1104,8 +1155,8 @@
         <v>444</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
       <c r="K2" s="11"/>
       <c r="L2" s="7">
         <v>420</v>
@@ -1121,187 +1172,187 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="21">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28"/>
+      <c r="B4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4" s="10" t="s">
+      <c r="D4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
+      <c r="B5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C5" s="10">
         <v>2</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-    </row>
-    <row r="5" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="D5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C6" s="10">
         <v>3</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="D6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C7" s="11">
         <v>4</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="16">
-        <v>5</v>
-      </c>
       <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="17"/>
+      <c r="F7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="10"/>
       <c r="I7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="16"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="13" t="s">
         <v>18</v>
       </c>
@@ -1318,16 +1369,16 @@
     <row r="8" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="28"/>
       <c r="B8" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>18</v>
+      <c r="E8" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>18</v>
@@ -1339,8 +1390,8 @@
       <c r="I8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="13" t="s">
-        <v>18</v>
+      <c r="J8" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="K8" s="16"/>
       <c r="L8" s="13" t="s">
@@ -1357,14 +1408,12 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>36</v>
-      </c>
+      <c r="A9" s="29"/>
       <c r="B9" s="16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" s="16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
@@ -1379,8 +1428,8 @@
         <v>18</v>
       </c>
       <c r="H9" s="17"/>
-      <c r="I9" s="13" t="s">
-        <v>18</v>
+      <c r="I9" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>18</v>
@@ -1400,33 +1449,35 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
-      <c r="B10" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="20">
-        <v>8</v>
+      <c r="A10" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="16">
+        <v>7</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>17</v>
+      <c r="E10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="H10" s="17"/>
-      <c r="I10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="20"/>
+      <c r="I10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="16"/>
       <c r="L10" s="13" t="s">
         <v>18</v>
       </c>
@@ -1442,69 +1493,104 @@
     </row>
     <row r="11" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28"/>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="20">
+        <v>8</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="20"/>
+      <c r="L11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
+      <c r="B12" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C12" s="16">
         <v>9</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O11" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="D12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="K14" s="9"/>
@@ -2184,18 +2270,24 @@
       <c r="M126" s="9"/>
       <c r="N126" s="9"/>
     </row>
+    <row r="127" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K127" s="9"/>
+      <c r="L127" s="9"/>
+      <c r="M127" s="9"/>
+      <c r="N127" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A13:O13"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>